<commit_message>
valores de br espelhados na coluna de eof, ajustes na pilha do analisador sintatico
</commit_message>
<xml_diff>
--- a/src/testes/EnumeracaoDeTerminais.xlsx
+++ b/src/testes/EnumeracaoDeTerminais.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2430" windowWidth="16200" windowHeight="24405"/>
+    <workbookView xWindow="0" yWindow="3645" windowWidth="16200" windowHeight="24405"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -566,8 +566,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A53" workbookViewId="0">
-      <selection sqref="A1:A56"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>